<commit_message>
random study session knapsack implementation almost done
</commit_message>
<xml_diff>
--- a/zz Non-LeetCode/Random Study Session 1/knapsack.xlsx
+++ b/zz Non-LeetCode/Random Study Session 1/knapsack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\zz Non-LeetCode\Random Study Session 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C800BE35-79D7-464B-BFE2-A9A30512A5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE881DC-CF3B-40A2-A72F-BA086E49E2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,8 +385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:AC51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,9 +1182,6 @@
       <c r="AB32" s="1">
         <v>18</v>
       </c>
-      <c r="AC32" s="1">
-        <v>18</v>
-      </c>
     </row>
     <row r="33" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
@@ -1245,7 +1242,7 @@
         <v>18</v>
       </c>
       <c r="AC33" s="1">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="4:29" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DYING on this problem omg
</commit_message>
<xml_diff>
--- a/zz Non-LeetCode/Random Study Session 1/knapsack.xlsx
+++ b/zz Non-LeetCode/Random Study Session 1/knapsack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\zz Non-LeetCode\Random Study Session 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B386E82-91E4-467D-A577-F1CDD5BE3990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FF3C37-E628-47DB-BA73-38504045A1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="69">
   <si>
     <t>Size</t>
   </si>
@@ -215,12 +216,69 @@
   <si>
     <t>aae</t>
   </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>Abcde</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AbcDE</t>
+  </si>
+  <si>
+    <t>AFDE</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>beFgH</t>
+  </si>
+  <si>
+    <t>EFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e </t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>tot</t>
+  </si>
+  <si>
+    <t>frced</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,8 +293,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFD4E4F9"/>
+      <name val="Var(--font-family-input)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +356,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -298,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -334,6 +417,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +718,7 @@
       <selection activeCell="AJ25" sqref="AJ25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="4.7109375" style="1"/>
     <col min="5" max="5" width="4.7109375" style="1" customWidth="1"/>
@@ -629,7 +727,7 @@
     <col min="18" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:28">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -643,7 +741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:28">
       <c r="B4" s="1">
         <v>0</v>
       </c>
@@ -664,7 +762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:28">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -709,7 +807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:28">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -754,7 +852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:28">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -812,7 +910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:28">
       <c r="I8" s="1" t="s">
         <v>4</v>
       </c>
@@ -844,7 +942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:28">
       <c r="D12" s="1">
         <v>1</v>
       </c>
@@ -921,7 +1019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:28">
       <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
@@ -971,7 +1069,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:28">
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1021,7 +1119,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:28">
       <c r="C15" s="1">
         <v>0</v>
       </c>
@@ -1071,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:28">
       <c r="C16" s="1">
         <v>1</v>
       </c>
@@ -1121,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:29">
       <c r="C17" s="1">
         <v>2</v>
       </c>
@@ -1171,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:29">
       <c r="C18" s="1">
         <v>3</v>
       </c>
@@ -1221,12 +1319,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:29">
       <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:29">
       <c r="D23" s="1">
         <v>7</v>
       </c>
@@ -1240,27 +1338,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:29">
       <c r="C24" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:29">
       <c r="C25" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:29">
       <c r="C26" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:29">
       <c r="C27" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:29">
       <c r="E31" s="1">
         <v>1</v>
       </c>
@@ -1337,7 +1435,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:29">
       <c r="D32" s="1" t="s">
         <v>6</v>
       </c>
@@ -1414,7 +1512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:29">
       <c r="D33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1476,17 +1574,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:29">
       <c r="D34" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:29">
       <c r="D35" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:29">
       <c r="D36" s="1">
         <v>2</v>
       </c>
@@ -1536,7 +1634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:29">
       <c r="D37" s="1">
         <v>3</v>
       </c>
@@ -1562,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:29">
       <c r="D39" s="1" t="s">
         <v>2</v>
       </c>
@@ -1576,7 +1674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:29">
       <c r="D40" s="1">
         <v>2</v>
       </c>
@@ -1591,7 +1689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:29">
       <c r="D41" s="1">
         <v>1</v>
       </c>
@@ -1606,7 +1704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:29">
       <c r="D42" s="1">
         <v>0</v>
       </c>
@@ -1621,7 +1719,7 @@
         <v>8.6363636363636367</v>
       </c>
     </row>
-    <row r="43" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:29">
       <c r="D43" s="1">
         <v>3</v>
       </c>
@@ -1636,13 +1734,13 @@
         <v>8.5714285714285712</v>
       </c>
     </row>
-    <row r="48" spans="4:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:29">
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="17:17">
       <c r="Q49" s="2"/>
     </row>
-    <row r="51" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="17:17">
       <c r="Q51" s="2"/>
     </row>
   </sheetData>
@@ -1658,12 +1756,12 @@
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1674,7 +1772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1682,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -1690,7 +1788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -1698,7 +1796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -1706,7 +1804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="D13" s="1">
         <v>1</v>
       </c>
@@ -1753,7 +1851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="C14" s="1">
         <v>1</v>
       </c>
@@ -1767,7 +1865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="C15" s="1">
         <v>2</v>
       </c>
@@ -1781,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="C16" s="1">
         <v>4</v>
       </c>
@@ -1792,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5">
       <c r="C17" s="1">
         <v>5</v>
       </c>
@@ -1803,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5">
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1814,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5">
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
@@ -1839,12 +1937,12 @@
       <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:24">
       <c r="E8" s="3">
         <v>0</v>
       </c>
@@ -1867,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="5:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:24">
       <c r="R9" s="1">
         <v>0</v>
       </c>
@@ -1890,7 +1988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="5:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:24">
       <c r="E10" s="1">
         <v>0</v>
       </c>
@@ -1934,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="5:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:24">
       <c r="R11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1957,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="5:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:24">
       <c r="E12" s="1">
         <v>0</v>
       </c>
@@ -1980,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="5:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:24">
       <c r="E14" s="1">
         <v>0</v>
       </c>
@@ -2024,7 +2122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="5:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:24">
       <c r="R15" s="1" t="s">
         <v>8</v>
       </c>
@@ -2047,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="5:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:24">
       <c r="E16" s="1">
         <v>0</v>
       </c>
@@ -2070,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:11">
       <c r="E18" s="1">
         <v>0</v>
       </c>
@@ -2093,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:11">
       <c r="I27" s="1">
         <v>8800</v>
       </c>
@@ -2105,13 +2203,13 @@
         <v>800</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:11">
       <c r="K28" s="1">
         <f>K27*4.8</f>
         <v>3840</v>
       </c>
     </row>
-    <row r="33" spans="5:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:31">
       <c r="E33" s="1">
         <v>0</v>
       </c>
@@ -2173,7 +2271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="5:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:31">
       <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
@@ -2235,7 +2333,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="5:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:31">
       <c r="S41" s="3">
         <v>1</v>
       </c>
@@ -2264,7 +2362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="5:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:31">
       <c r="S42" s="3">
         <v>0</v>
       </c>
@@ -2287,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="5:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:31">
       <c r="S43" s="3">
         <v>1</v>
       </c>
@@ -2316,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="5:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:31">
       <c r="S44" s="3">
         <v>0</v>
       </c>
@@ -2336,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="5:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:31">
       <c r="S45" s="1">
         <v>0</v>
       </c>
@@ -2356,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="5:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:31">
       <c r="S46" s="1">
         <v>0</v>
       </c>
@@ -2390,12 +2488,12 @@
       <selection activeCell="AB12" sqref="AB12:AC12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="7:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:35">
       <c r="G8" s="1">
         <v>0</v>
       </c>
@@ -2439,7 +2537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="7:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="7:35">
       <c r="G9" s="3">
         <v>7</v>
       </c>
@@ -2513,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="7:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:35">
       <c r="G10" s="3">
         <v>2</v>
       </c>
@@ -2557,7 +2655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="7:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:35">
       <c r="G11" s="1">
         <v>1</v>
       </c>
@@ -2601,7 +2699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="7:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:35">
       <c r="G12" s="1">
         <v>1</v>
       </c>
@@ -2645,7 +2743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="7:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:35">
       <c r="G13" s="1">
         <v>1</v>
       </c>
@@ -2689,7 +2787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="7:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="7:35">
       <c r="G14" s="1">
         <v>1</v>
       </c>
@@ -2733,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:40">
       <c r="G17" s="3">
         <v>4</v>
       </c>
@@ -2771,7 +2869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:40">
       <c r="G18" s="1">
         <v>1</v>
       </c>
@@ -2809,7 +2907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:40">
       <c r="G19" s="1">
         <v>1</v>
       </c>
@@ -2847,7 +2945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:40">
       <c r="G20" s="1">
         <v>1</v>
       </c>
@@ -2885,7 +2983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:40">
       <c r="G25" s="3">
         <v>0</v>
       </c>
@@ -2908,7 +3006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:40">
       <c r="E26" s="1" t="s">
         <v>12</v>
       </c>
@@ -2958,7 +3056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:40">
       <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
@@ -3023,7 +3121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:40">
       <c r="AJ28" s="1">
         <v>1</v>
       </c>
@@ -3040,7 +3138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:40">
       <c r="AC29" s="1">
         <v>0</v>
       </c>
@@ -3057,7 +3155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:40">
       <c r="AC30" s="1">
         <v>2</v>
       </c>
@@ -3089,7 +3187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="5:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:40">
       <c r="AC32" s="1">
         <v>1</v>
       </c>
@@ -3119,14 +3217,14 @@
       <selection activeCell="V121" sqref="V121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="34" width="4.7109375" style="1"/>
     <col min="35" max="35" width="4.7109375" style="1" customWidth="1"/>
     <col min="36" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:54">
       <c r="AV2" s="5">
         <v>7</v>
       </c>
@@ -3149,7 +3247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="7:54">
       <c r="AV3" s="1">
         <v>1</v>
       </c>
@@ -3157,7 +3255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:54">
       <c r="AX4" s="1">
         <v>5</v>
       </c>
@@ -3165,7 +3263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:54">
       <c r="AW5" s="1">
         <v>2</v>
       </c>
@@ -3173,7 +3271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:54">
       <c r="Z6" s="1">
         <v>7</v>
       </c>
@@ -3202,7 +3300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:54">
       <c r="AX7" s="1">
         <v>3</v>
       </c>
@@ -3210,7 +3308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:54">
       <c r="G10" s="5">
         <v>1</v>
       </c>
@@ -3275,7 +3373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:54">
       <c r="K11" s="1">
         <v>7</v>
       </c>
@@ -3298,7 +3396,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:54">
       <c r="G12" s="1">
         <v>7</v>
       </c>
@@ -3321,7 +3419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:54">
       <c r="G13" s="5">
         <v>7</v>
       </c>
@@ -3374,7 +3472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="7:54">
       <c r="H14" s="1">
         <v>4</v>
       </c>
@@ -3397,7 +3495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="7:54">
       <c r="I15" s="1">
         <v>1</v>
       </c>
@@ -3411,7 +3509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="7:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:54">
       <c r="J16" s="1">
         <v>6</v>
       </c>
@@ -3442,7 +3540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:44">
       <c r="G17" s="5">
         <v>7</v>
       </c>
@@ -3489,7 +3587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:44">
       <c r="G18" s="1">
         <v>1</v>
       </c>
@@ -3500,7 +3598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:44">
       <c r="H19" s="1">
         <v>2</v>
       </c>
@@ -3511,7 +3609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:44">
       <c r="I20" s="1">
         <v>3</v>
       </c>
@@ -3522,7 +3620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:44">
       <c r="J21" s="1">
         <v>4</v>
       </c>
@@ -3536,7 +3634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:44">
       <c r="K22" s="1">
         <v>5</v>
       </c>
@@ -3596,7 +3694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:44">
       <c r="Z23" s="6">
         <v>0</v>
       </c>
@@ -3643,7 +3741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:44">
       <c r="Y24" s="1" t="s">
         <v>15</v>
       </c>
@@ -3697,7 +3795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:44">
       <c r="Z25" s="10">
         <v>7</v>
       </c>
@@ -3720,7 +3818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:44">
       <c r="AI26" s="7">
         <f>AI23-AI24</f>
         <v>-2</v>
@@ -3750,97 +3848,97 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:44">
       <c r="AI28" s="5">
-        <f>HLOOKUP(AI24+AI26,$Z$24:$AF$25,2,FALSE)</f>
+        <f t="shared" ref="AI28:AO28" si="3">HLOOKUP(AI24+AI26,$Z$24:$AF$25,2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="AJ28" s="5">
-        <f>HLOOKUP(AJ24+AJ26,$Z$24:$AF$25,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="AK28" s="5">
-        <f>HLOOKUP(AK24+AK26,$Z$24:$AF$25,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AL28" s="5">
-        <f>HLOOKUP(AL24+AL26,$Z$24:$AF$25,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AM28" s="5">
-        <f>HLOOKUP(AM24+AM26,$Z$24:$AF$25,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="AN28" s="5">
-        <f>HLOOKUP(AN24+AN26,$Z$24:$AF$25,2,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="AO28" s="5">
-        <f>HLOOKUP(AO24+AO26,$Z$24:$AF$25,2,FALSE)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="7:44" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="7:44">
       <c r="AI29" s="8">
         <f>HLOOKUP(AI28,$AI$23:$AO$26,4,FALSE)</f>
         <v>6</v>
       </c>
       <c r="AJ29" s="8">
-        <f t="shared" ref="AJ29:AO29" si="3">HLOOKUP(AJ28,$AI$23:$AO$26,4,FALSE)</f>
+        <f t="shared" ref="AJ29:AO29" si="4">HLOOKUP(AJ28,$AI$23:$AO$26,4,FALSE)</f>
         <v>2</v>
       </c>
       <c r="AK29" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="AL29" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="AM29" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="AN29" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AO29" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
     </row>
-    <row r="31" spans="7:44" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:44">
       <c r="AI31" s="9">
-        <f>AI29+AI26</f>
+        <f t="shared" ref="AI31:AO31" si="5">AI29+AI26</f>
         <v>4</v>
       </c>
       <c r="AJ31" s="9">
-        <f>AJ29+AJ26</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AK31" s="9">
-        <f>AK29+AK26</f>
+        <f t="shared" si="5"/>
         <v>-4</v>
       </c>
       <c r="AL31" s="9">
-        <f>AL29+AL26</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AM31" s="9">
-        <f>AM29+AM26</f>
+        <f t="shared" si="5"/>
         <v>-4</v>
       </c>
       <c r="AN31" s="9">
-        <f>AN29+AN26</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO31" s="9">
-        <f>AO29+AO26</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="5:41" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="5:41">
       <c r="F34" s="6">
         <v>0</v>
       </c>
@@ -3884,7 +3982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:41">
       <c r="E35" s="1" t="s">
         <v>15</v>
       </c>
@@ -3934,7 +4032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:41">
       <c r="F36" s="5">
         <v>4</v>
       </c>
@@ -4020,7 +4118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:41">
       <c r="Z37" s="6">
         <v>0</v>
       </c>
@@ -4067,33 +4165,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:41">
       <c r="O38" s="1">
         <f>O35-O36</f>
         <v>-3</v>
       </c>
       <c r="P38" s="1">
-        <f t="shared" ref="P38:U38" si="4">P35-P36</f>
+        <f t="shared" ref="P38:U38" si="6">P35-P36</f>
         <v>0</v>
       </c>
       <c r="Q38" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R38" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="S38" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
       <c r="T38" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U38" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="Y38" s="1" t="s">
@@ -4142,7 +4240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:41">
       <c r="Z39" s="10">
         <v>1</v>
       </c>
@@ -4165,7 +4263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:41">
       <c r="AI40" s="7">
         <v>0</v>
       </c>
@@ -4188,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:41">
       <c r="F42" s="6">
         <v>0</v>
       </c>
@@ -4253,7 +4351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:41">
       <c r="E43" s="1" t="s">
         <v>15</v>
       </c>
@@ -4324,7 +4422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:41">
       <c r="F44" s="5">
         <v>5</v>
       </c>
@@ -4368,7 +4466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:41">
       <c r="AI45" s="9">
         <v>0</v>
       </c>
@@ -4391,37 +4489,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="5:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:41">
       <c r="O46" s="1">
         <f>O43-O44</f>
         <v>-4</v>
       </c>
       <c r="P46" s="1">
-        <f t="shared" ref="P46:U46" si="5">P43-P44</f>
+        <f t="shared" ref="P46:U46" si="7">P43-P44</f>
         <v>0</v>
       </c>
       <c r="Q46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-3</v>
       </c>
       <c r="S46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="T46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U46" s="1">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="16:24" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="16:24">
       <c r="P69" s="1">
         <v>2</v>
       </c>
@@ -4441,7 +4539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="16:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="16:24">
       <c r="P70" s="1">
         <v>1</v>
       </c>
@@ -4464,7 +4562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="16:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="16:24">
       <c r="P71" s="1">
         <v>1</v>
       </c>
@@ -4487,7 +4585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="16:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="16:24">
       <c r="P72" s="1">
         <v>1</v>
       </c>
@@ -4510,12 +4608,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="16:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="16:24">
       <c r="V73" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="16:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="16:24">
       <c r="P79" s="1">
         <v>2</v>
       </c>
@@ -4535,7 +4633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="16:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="16:24">
       <c r="P80" s="1">
         <v>1</v>
       </c>
@@ -4558,7 +4656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:45">
       <c r="P81" s="1">
         <v>1</v>
       </c>
@@ -4578,7 +4676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:45">
       <c r="P82" s="1">
         <v>1</v>
       </c>
@@ -4601,7 +4699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:45">
       <c r="P83" s="1">
         <v>1</v>
       </c>
@@ -4624,29 +4722,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:45">
       <c r="AB94" s="1">
         <f>AB96</f>
         <v>3</v>
       </c>
       <c r="AC94" s="1">
-        <f t="shared" ref="AC94:AG94" si="6">AC96</f>
+        <f t="shared" ref="AC94:AG94" si="8">AC96</f>
         <v>4</v>
       </c>
       <c r="AD94" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AE94" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AF94" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AG94" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="AK94" s="1">
@@ -4671,7 +4769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:45">
       <c r="D95" s="1">
         <v>1</v>
       </c>
@@ -4745,7 +4843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:45">
       <c r="H96" s="1">
         <v>6</v>
       </c>
@@ -4798,7 +4896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:45">
       <c r="G97" s="1">
         <v>6</v>
       </c>
@@ -4833,7 +4931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:45">
       <c r="D98" s="1">
         <v>1</v>
       </c>
@@ -4872,23 +4970,23 @@
         <v>5</v>
       </c>
       <c r="AC98" s="1">
-        <f t="shared" ref="AC98:AG98" si="7">HLOOKUP(AC95,$AB$94:$AG$96,2,FALSE)</f>
+        <f t="shared" ref="AC98:AG98" si="9">HLOOKUP(AC95,$AB$94:$AG$96,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="AD98" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AE98" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AF98" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AG98" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AK98" s="1">
@@ -4904,7 +5002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:45">
       <c r="L99" s="1">
         <v>5</v>
       </c>
@@ -4945,7 +5043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:45">
       <c r="L100" s="1">
         <v>6</v>
       </c>
@@ -4981,23 +5079,23 @@
         <v>4</v>
       </c>
       <c r="AC100" s="1">
-        <f t="shared" ref="AC100:AG100" si="8">AC98-AC95</f>
+        <f t="shared" ref="AC100:AG100" si="10">AC98-AC95</f>
         <v>4</v>
       </c>
       <c r="AD100" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="AE100" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="AF100" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="AG100" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="AO100" s="1">
@@ -5007,7 +5105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:45">
       <c r="O101" s="1">
         <v>3</v>
       </c>
@@ -5021,7 +5119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:45">
       <c r="P102" s="1">
         <v>4</v>
       </c>
@@ -5035,7 +5133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:45">
       <c r="Q103" s="1">
         <v>5</v>
       </c>
@@ -5049,7 +5147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:45">
       <c r="R104" s="1">
         <v>6</v>
       </c>
@@ -5075,7 +5173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:45">
       <c r="S105" s="1">
         <v>1</v>
       </c>
@@ -5083,7 +5181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:45">
       <c r="O106" s="1">
         <v>3</v>
       </c>
@@ -5103,7 +5201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="4:45" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:45">
       <c r="V112" s="1">
         <v>2</v>
       </c>
@@ -5123,7 +5221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="22:30" x14ac:dyDescent="0.25">
+    <row r="113" spans="22:30">
       <c r="W113" s="1">
         <v>1</v>
       </c>
@@ -5137,7 +5235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="22:30" x14ac:dyDescent="0.25">
+    <row r="114" spans="22:30">
       <c r="V114" s="1">
         <v>1</v>
       </c>
@@ -5148,7 +5246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="22:30" x14ac:dyDescent="0.25">
+    <row r="115" spans="22:30">
       <c r="V115" s="1">
         <v>1</v>
       </c>
@@ -5168,7 +5266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="22:30" x14ac:dyDescent="0.25">
+    <row r="116" spans="22:30">
       <c r="X116" s="1">
         <v>3</v>
       </c>
@@ -5182,7 +5280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="22:30" x14ac:dyDescent="0.25">
+    <row r="117" spans="22:30">
       <c r="V117" s="1">
         <v>1</v>
       </c>
@@ -5199,7 +5297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="22:30" x14ac:dyDescent="0.25">
+    <row r="118" spans="22:30">
       <c r="Y118" s="1">
         <v>4</v>
       </c>
@@ -5220,14 +5318,14 @@
       <selection activeCell="K27" sqref="H27:K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="11" width="4.7109375" style="1"/>
     <col min="12" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:13">
       <c r="G11" s="1">
         <v>1</v>
       </c>
@@ -5250,7 +5348,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:14">
       <c r="H18" s="1">
         <v>10</v>
       </c>
@@ -5273,7 +5371,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:14">
       <c r="I19" s="1" t="s">
         <v>17</v>
       </c>
@@ -5281,7 +5379,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:14">
       <c r="H21" s="1">
         <v>10</v>
       </c>
@@ -5304,7 +5402,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:14">
       <c r="K22" s="1" t="s">
         <v>17</v>
       </c>
@@ -5312,7 +5410,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:14">
       <c r="H24" s="1">
         <v>10</v>
       </c>
@@ -5335,7 +5433,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:14">
       <c r="K25" s="1" t="s">
         <v>19</v>
       </c>
@@ -5343,7 +5441,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:14">
       <c r="H27" s="1">
         <v>10</v>
       </c>
@@ -5366,7 +5464,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:14">
       <c r="K28" s="1" t="s">
         <v>19</v>
       </c>
@@ -5387,9 +5485,9 @@
       <selection activeCell="K30" sqref="F30:K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="22" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:27">
       <c r="K22">
         <v>2</v>
       </c>
@@ -5409,7 +5507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:27">
       <c r="F26">
         <v>1</v>
       </c>
@@ -5420,7 +5518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:27">
       <c r="F27">
         <v>1</v>
       </c>
@@ -5434,7 +5532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:27">
       <c r="M29">
         <v>1</v>
       </c>
@@ -5472,7 +5570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:27">
       <c r="M30">
         <v>1</v>
       </c>
@@ -5510,7 +5608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:27">
       <c r="M31">
         <v>1</v>
       </c>
@@ -5548,7 +5646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="17:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="17:30">
       <c r="Q33" t="s">
         <v>20</v>
       </c>
@@ -5571,18 +5669,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF082638-1CAB-438C-807C-7C5CDDCFB1E8}">
   <dimension ref="G12:AX142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O118" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="O121" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="AE142" sqref="AE142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="19" width="4.7109375" style="1"/>
     <col min="20" max="20" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:14">
       <c r="H12" s="1">
         <v>-2</v>
       </c>
@@ -5605,7 +5703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:14">
       <c r="H13" s="1">
         <v>-2</v>
       </c>
@@ -5625,7 +5723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="20" spans="17:50">
       <c r="AK20" s="1">
         <v>1</v>
       </c>
@@ -5645,7 +5743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="21" spans="17:50">
       <c r="R21" s="1">
         <v>-2</v>
       </c>
@@ -5674,7 +5772,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="22" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="17:50">
       <c r="Q22" s="1">
         <v>1</v>
       </c>
@@ -5685,7 +5783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="23" spans="17:50">
       <c r="Q23" s="1">
         <v>2</v>
       </c>
@@ -5699,7 +5797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="24" spans="17:50">
       <c r="Q24" s="1">
         <v>3</v>
       </c>
@@ -5713,7 +5811,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="25" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="25" spans="17:50">
       <c r="Q25" s="1">
         <v>4</v>
       </c>
@@ -5724,17 +5822,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="17:50">
       <c r="Q26" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="27" spans="17:50">
       <c r="Q27" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="29" spans="17:50">
       <c r="AG29" s="1">
         <v>2</v>
       </c>
@@ -5772,7 +5870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="30" spans="17:50">
       <c r="W30" s="1">
         <v>2</v>
       </c>
@@ -5795,7 +5893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="31" spans="17:50">
       <c r="V31" s="1">
         <v>3</v>
       </c>
@@ -5815,7 +5913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="17:50" x14ac:dyDescent="0.25">
+    <row r="32" spans="17:50">
       <c r="V32" s="1">
         <v>7</v>
       </c>
@@ -5832,7 +5930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="22:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="22:47">
       <c r="V33" s="1">
         <v>4</v>
       </c>
@@ -5852,7 +5950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="22:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="22:47">
       <c r="V34" s="1">
         <v>6</v>
       </c>
@@ -5869,7 +5967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="22:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="22:47">
       <c r="V35" s="1">
         <v>5</v>
       </c>
@@ -5889,7 +5987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="22:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="22:47">
       <c r="AF36" s="1">
         <v>1</v>
       </c>
@@ -5900,7 +5998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="22:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="22:47">
       <c r="AT37" s="1">
         <v>5</v>
       </c>
@@ -5908,12 +6006,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="22:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="22:47">
       <c r="AT38" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:47">
       <c r="I51" s="1">
         <v>-2</v>
       </c>
@@ -5988,7 +6086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:47">
       <c r="H52" s="1">
         <v>-2</v>
       </c>
@@ -6041,7 +6139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:47">
       <c r="H53" s="1">
         <v>1</v>
       </c>
@@ -6067,7 +6165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:47">
       <c r="H54" s="1">
         <v>3</v>
       </c>
@@ -6084,7 +6182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:47">
       <c r="H55" s="1">
         <v>-4</v>
       </c>
@@ -6101,7 +6199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:47">
       <c r="H56" s="1">
         <v>5</v>
       </c>
@@ -6112,7 +6210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:47">
       <c r="H57" s="1">
         <v>6</v>
       </c>
@@ -6132,22 +6230,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:47">
       <c r="AL58" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:47">
       <c r="AL59" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="8:47" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:47">
       <c r="AL60" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="7:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:21">
       <c r="H69" s="1">
         <v>5</v>
       </c>
@@ -6164,7 +6262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="7:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:21">
       <c r="H74" s="1">
         <v>0</v>
       </c>
@@ -6199,7 +6297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="7:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:21">
       <c r="H75" s="1">
         <v>-2</v>
       </c>
@@ -6234,7 +6332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="7:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:21">
       <c r="G76" s="1" t="s">
         <v>5</v>
       </c>
@@ -6266,7 +6364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="7:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:21">
       <c r="G77" s="1" t="s">
         <v>14</v>
       </c>
@@ -6298,7 +6396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="7:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:31">
       <c r="G84" s="1">
         <v>1</v>
       </c>
@@ -6318,7 +6416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="7:31" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:31">
       <c r="G85" s="1">
         <v>1</v>
       </c>
@@ -6338,7 +6436,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="7:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:31">
       <c r="P91" s="1">
         <v>1</v>
       </c>
@@ -6349,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="7:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:31">
       <c r="O92" s="1">
         <v>1</v>
       </c>
@@ -6366,7 +6464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="7:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:31">
       <c r="N93" s="1">
         <v>1</v>
       </c>
@@ -6389,7 +6487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="7:31" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:31">
       <c r="M94" s="1">
         <v>1</v>
       </c>
@@ -6418,7 +6516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="7:31" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:31">
       <c r="L95" s="1">
         <v>1</v>
       </c>
@@ -6453,7 +6551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="100" spans="19:46">
       <c r="S100" s="4">
         <v>0</v>
       </c>
@@ -6464,7 +6562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="101" spans="19:46">
       <c r="S101" s="4">
         <v>1</v>
       </c>
@@ -6475,7 +6573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="102" spans="19:46">
       <c r="S102" s="11">
         <v>2</v>
       </c>
@@ -6486,7 +6584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="103" spans="19:46">
       <c r="S103" s="11">
         <v>3</v>
       </c>
@@ -6497,7 +6595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="104" spans="19:46">
       <c r="S104" s="1">
         <v>4</v>
       </c>
@@ -6508,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="105" spans="19:46">
       <c r="S105" s="1">
         <v>5</v>
       </c>
@@ -6519,7 +6617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="106" spans="19:46">
       <c r="S106" s="1">
         <v>6</v>
       </c>
@@ -6530,7 +6628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="107" spans="19:46">
       <c r="S107" s="1">
         <v>7</v>
       </c>
@@ -6541,7 +6639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="108" spans="19:46">
       <c r="S108" s="11">
         <v>8</v>
       </c>
@@ -6552,7 +6650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="109" spans="19:46">
       <c r="S109" s="11">
         <v>9</v>
       </c>
@@ -6566,7 +6664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="110" spans="19:46">
       <c r="S110" s="11">
         <v>10</v>
       </c>
@@ -6577,7 +6675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="111" spans="19:46">
       <c r="S111" s="11">
         <v>11</v>
       </c>
@@ -6610,7 +6708,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="112" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="112" spans="19:46">
       <c r="S112" s="11">
         <v>12</v>
       </c>
@@ -6642,7 +6740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="113" spans="19:46">
       <c r="S113" s="11">
         <v>13</v>
       </c>
@@ -6674,7 +6772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="114" spans="19:46">
       <c r="S114" s="11">
         <v>14</v>
       </c>
@@ -6706,7 +6804,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="115" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="115" spans="19:46">
       <c r="S115" s="11">
         <v>15</v>
       </c>
@@ -6717,7 +6815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="116" spans="19:46">
       <c r="S116" s="1">
         <v>16</v>
       </c>
@@ -6725,17 +6823,17 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="117" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="117" spans="19:46">
       <c r="S117" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="118" spans="19:46">
       <c r="S118" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="119" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="119" spans="19:46">
       <c r="S119" s="1">
         <v>31</v>
       </c>
@@ -6743,7 +6841,7 @@
         <v>11111</v>
       </c>
     </row>
-    <row r="120" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="120" spans="19:46">
       <c r="S120" s="11">
         <v>32</v>
       </c>
@@ -6754,7 +6852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="121" spans="19:46">
       <c r="S121" s="11" t="s">
         <v>22</v>
       </c>
@@ -6765,7 +6863,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="122" spans="19:46">
       <c r="S122" s="11" t="s">
         <v>22</v>
       </c>
@@ -6785,7 +6883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="123" spans="19:46">
       <c r="S123" s="11">
         <v>64</v>
       </c>
@@ -6824,7 +6922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="124" spans="19:46">
       <c r="AE124" s="1" t="s">
         <v>16</v>
       </c>
@@ -6838,7 +6936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="125" spans="19:46">
       <c r="AE125" s="1" t="s">
         <v>17</v>
       </c>
@@ -6852,7 +6950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="126" spans="19:46">
       <c r="AE126" s="1" t="s">
         <v>18</v>
       </c>
@@ -6866,7 +6964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="127" spans="19:46">
       <c r="AE127" s="1" t="s">
         <v>23</v>
       </c>
@@ -6880,7 +6978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="19:46" x14ac:dyDescent="0.25">
+    <row r="128" spans="19:46">
       <c r="AE128" s="1" t="s">
         <v>32</v>
       </c>
@@ -6896,7 +6994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="131" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="131" spans="22:44">
       <c r="V131" s="1" t="s">
         <v>9</v>
       </c>
@@ -6928,7 +7026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="132" spans="22:44">
       <c r="W132" s="1" t="s">
         <v>16</v>
       </c>
@@ -6942,7 +7040,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="133" spans="22:44">
       <c r="W133" s="1" t="s">
         <v>17</v>
       </c>
@@ -6953,7 +7051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="134" spans="22:44">
       <c r="W134" s="1" t="s">
         <v>18</v>
       </c>
@@ -6961,12 +7059,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="135" spans="22:44">
       <c r="W135" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="137" spans="22:44">
       <c r="AN137" s="1" t="s">
         <v>9</v>
       </c>
@@ -6983,7 +7081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="138" spans="22:44">
       <c r="V138" s="1" t="s">
         <v>26</v>
       </c>
@@ -7036,7 +7134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="139" spans="22:44">
       <c r="V139" s="1" t="s">
         <v>27</v>
       </c>
@@ -7077,7 +7175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="140" spans="22:44">
       <c r="V140" s="1" t="s">
         <v>28</v>
       </c>
@@ -7103,7 +7201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="141" spans="22:44">
       <c r="V141" s="1" t="s">
         <v>24</v>
       </c>
@@ -7111,7 +7209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="142" spans="22:44" x14ac:dyDescent="0.25">
+    <row r="142" spans="22:44">
       <c r="V142" s="1" t="s">
         <v>34</v>
       </c>
@@ -7119,4 +7217,1954 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32FE7F7-B5E4-4E8D-81E0-4C33AFBF73DF}">
+  <dimension ref="C7:AI101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AD99" sqref="AD99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="4.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="9:31">
+      <c r="I7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="9:31">
+      <c r="I8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="9:31">
+      <c r="I9" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="9:31">
+      <c r="I12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="9:31">
+      <c r="I13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="9:31">
+      <c r="M14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="9:31">
+      <c r="M15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1">
+        <v>1</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0</v>
+      </c>
+      <c r="X15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="9:31">
+      <c r="T16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0</v>
+      </c>
+      <c r="W16" s="1">
+        <v>1</v>
+      </c>
+      <c r="X16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="9:31">
+      <c r="T17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0</v>
+      </c>
+      <c r="W17" s="1">
+        <v>0</v>
+      </c>
+      <c r="X17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="9:31">
+      <c r="I25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="9:31">
+      <c r="I26" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>0</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U26" s="1">
+        <v>0</v>
+      </c>
+      <c r="V26" s="1">
+        <v>1</v>
+      </c>
+      <c r="W26" s="1">
+        <v>0</v>
+      </c>
+      <c r="X26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="9:31">
+      <c r="L27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U27" s="1">
+        <v>0</v>
+      </c>
+      <c r="V27" s="1">
+        <v>0</v>
+      </c>
+      <c r="W27" s="1">
+        <v>1</v>
+      </c>
+      <c r="X27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="9:31">
+      <c r="L28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U28" s="1">
+        <v>0</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0</v>
+      </c>
+      <c r="X28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="9:31">
+      <c r="U32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="4:35">
+      <c r="T33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U33" s="1">
+        <v>0</v>
+      </c>
+      <c r="V33" s="1">
+        <v>1</v>
+      </c>
+      <c r="W33" s="1">
+        <v>0</v>
+      </c>
+      <c r="X33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:35">
+      <c r="T34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U34" s="1">
+        <v>0</v>
+      </c>
+      <c r="V34" s="1">
+        <v>0</v>
+      </c>
+      <c r="W34" s="1">
+        <v>1</v>
+      </c>
+      <c r="X34" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="4:35">
+      <c r="T35" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="4:35">
+      <c r="U37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:35">
+      <c r="T38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U38" s="1">
+        <v>0</v>
+      </c>
+      <c r="V38" s="1">
+        <v>1</v>
+      </c>
+      <c r="W38" s="1">
+        <v>0</v>
+      </c>
+      <c r="X38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="4:35">
+      <c r="T39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U39" s="1">
+        <v>0</v>
+      </c>
+      <c r="V39" s="1">
+        <v>0</v>
+      </c>
+      <c r="W39" s="1">
+        <v>2</v>
+      </c>
+      <c r="X39" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:35">
+      <c r="T40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:35">
+      <c r="AB41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD41" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="4:35">
+      <c r="E44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE44" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="4:35">
+      <c r="D45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>2</v>
+      </c>
+      <c r="I45" s="1">
+        <v>2</v>
+      </c>
+      <c r="J45" s="1">
+        <v>2</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N45" s="1">
+        <v>0</v>
+      </c>
+      <c r="O45" s="1">
+        <v>1</v>
+      </c>
+      <c r="P45" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>0</v>
+      </c>
+      <c r="R45" s="1">
+        <v>2</v>
+      </c>
+      <c r="S45" s="1">
+        <v>2</v>
+      </c>
+      <c r="T45" s="1">
+        <v>2</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X45" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC45" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD45" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE45" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="4:35">
+      <c r="D46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N46" s="1">
+        <v>0</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X46" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="4:35">
+      <c r="D47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N47" s="1">
+        <v>0</v>
+      </c>
+      <c r="W47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X47" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:35">
+      <c r="M48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N48" s="1">
+        <v>0</v>
+      </c>
+      <c r="W48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="3:32">
+      <c r="N53" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="3:32">
+      <c r="M54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N54" s="14">
+        <v>2</v>
+      </c>
+      <c r="O54" s="14">
+        <v>2</v>
+      </c>
+      <c r="P54" s="14">
+        <v>2</v>
+      </c>
+      <c r="Q54" s="14">
+        <v>2</v>
+      </c>
+      <c r="R54" s="14">
+        <v>0</v>
+      </c>
+      <c r="S54" s="14">
+        <v>1</v>
+      </c>
+      <c r="T54" s="14">
+        <v>1</v>
+      </c>
+      <c r="U54" s="14">
+        <v>1</v>
+      </c>
+      <c r="V54" s="14">
+        <v>1</v>
+      </c>
+      <c r="W54" s="14">
+        <v>1</v>
+      </c>
+      <c r="X54" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:32">
+      <c r="M55" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N55" s="1">
+        <v>0</v>
+      </c>
+      <c r="O55" s="5">
+        <v>0</v>
+      </c>
+      <c r="P55" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="5">
+        <v>1</v>
+      </c>
+      <c r="R55" s="5">
+        <v>2</v>
+      </c>
+      <c r="S55" s="5">
+        <v>2</v>
+      </c>
+      <c r="T55" s="5">
+        <v>2</v>
+      </c>
+      <c r="U55" s="5">
+        <v>2</v>
+      </c>
+      <c r="V55" s="5">
+        <v>2</v>
+      </c>
+      <c r="W55" s="5">
+        <v>2</v>
+      </c>
+      <c r="X55" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="3:32">
+      <c r="M56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+    </row>
+    <row r="57" spans="3:32">
+      <c r="M57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="5"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+    </row>
+    <row r="60" spans="3:32">
+      <c r="D60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF60" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="3:32">
+      <c r="C61" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2</v>
+      </c>
+      <c r="F61" s="1">
+        <v>2</v>
+      </c>
+      <c r="G61" s="1">
+        <v>2</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
+        <v>1</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1">
+        <v>1</v>
+      </c>
+      <c r="L61" s="1">
+        <v>1</v>
+      </c>
+      <c r="M61" s="1">
+        <v>1</v>
+      </c>
+      <c r="N61" s="1">
+        <v>1</v>
+      </c>
+      <c r="O61" s="1">
+        <v>1</v>
+      </c>
+      <c r="P61" s="1">
+        <v>2</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T61" s="1">
+        <v>2</v>
+      </c>
+      <c r="U61" s="1">
+        <v>2</v>
+      </c>
+      <c r="V61" s="1">
+        <v>2</v>
+      </c>
+      <c r="W61" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD61" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF61" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="3:32">
+      <c r="C62" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1">
+        <v>2</v>
+      </c>
+      <c r="I62" s="1">
+        <v>2</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T62" s="1">
+        <v>0</v>
+      </c>
+      <c r="U62" s="1">
+        <v>0</v>
+      </c>
+      <c r="V62" s="1">
+        <v>0</v>
+      </c>
+      <c r="W62" s="1">
+        <v>1</v>
+      </c>
+      <c r="X62" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y62" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="3:32">
+      <c r="C63" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S63" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="3:32">
+      <c r="C64" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S64" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="3:33">
+      <c r="C65" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S65" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="3:33">
+      <c r="T70" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC70" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD70" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF70" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG70" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="3:33">
+      <c r="P71" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>2</v>
+      </c>
+      <c r="S71" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T71" s="1">
+        <v>1</v>
+      </c>
+      <c r="U71" s="1">
+        <v>1</v>
+      </c>
+      <c r="V71" s="1">
+        <v>1</v>
+      </c>
+      <c r="W71" s="1">
+        <v>1</v>
+      </c>
+      <c r="X71" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y71" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z71" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA71" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB71" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC71" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD71" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE71" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF71" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="3:33">
+      <c r="P72" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>2</v>
+      </c>
+      <c r="S72" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T72" s="1">
+        <v>2</v>
+      </c>
+      <c r="U72" s="1">
+        <v>2</v>
+      </c>
+      <c r="V72" s="1">
+        <v>2</v>
+      </c>
+      <c r="W72" s="1">
+        <v>2</v>
+      </c>
+      <c r="X72" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y72" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z72" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA72" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB72" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD72" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE72" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF72" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="3:33">
+      <c r="P73" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>1</v>
+      </c>
+      <c r="S73" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T73" s="1">
+        <v>1</v>
+      </c>
+      <c r="U73" s="1">
+        <v>1</v>
+      </c>
+      <c r="V73" s="1">
+        <v>1</v>
+      </c>
+      <c r="W73" s="1">
+        <v>1</v>
+      </c>
+      <c r="X73" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y73" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z73" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA73" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB73" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC73" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD73" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE73" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF73" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="3:33">
+      <c r="S74" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="T74" s="15">
+        <v>1</v>
+      </c>
+      <c r="U74" s="15">
+        <v>1</v>
+      </c>
+      <c r="V74" s="15">
+        <v>1</v>
+      </c>
+      <c r="W74" s="15">
+        <v>1</v>
+      </c>
+      <c r="X74" s="15">
+        <v>1</v>
+      </c>
+      <c r="Y74" s="15">
+        <v>1</v>
+      </c>
+      <c r="Z74" s="15">
+        <v>1</v>
+      </c>
+      <c r="AA74" s="15">
+        <v>1</v>
+      </c>
+      <c r="AB74" s="15">
+        <v>1</v>
+      </c>
+      <c r="AC74" s="15">
+        <v>1</v>
+      </c>
+      <c r="AD74" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE74" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF74" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG74" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="3:33">
+      <c r="S75" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="T75" s="15">
+        <v>2</v>
+      </c>
+      <c r="U75" s="15">
+        <v>2</v>
+      </c>
+      <c r="V75" s="15">
+        <v>2</v>
+      </c>
+      <c r="W75" s="15">
+        <v>2</v>
+      </c>
+      <c r="X75" s="15">
+        <v>1</v>
+      </c>
+      <c r="Y75" s="15">
+        <v>1</v>
+      </c>
+      <c r="Z75" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA75" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB75" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC75" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD75" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE75" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF75" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG75" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="3:33">
+      <c r="T78" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X78" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z78" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC78" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD78" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF78" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG78" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="79" spans="3:33">
+      <c r="S79" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T79" s="1">
+        <v>2</v>
+      </c>
+      <c r="U79" s="1">
+        <v>2</v>
+      </c>
+      <c r="V79" s="1">
+        <v>2</v>
+      </c>
+      <c r="W79" s="1">
+        <v>2</v>
+      </c>
+      <c r="X79" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y79" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z79" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA79" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB79" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC79" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD79" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE79" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF79" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG79" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="3:33">
+      <c r="S80" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T80" s="1">
+        <v>0</v>
+      </c>
+      <c r="U80" s="1">
+        <v>0</v>
+      </c>
+      <c r="V80" s="1">
+        <v>0</v>
+      </c>
+      <c r="W80" s="1">
+        <v>1</v>
+      </c>
+      <c r="X80" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y80" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="10:32">
+      <c r="S81" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="10:32">
+      <c r="S82" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="10:32">
+      <c r="S83" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="86" spans="10:32">
+      <c r="J86" s="17"/>
+      <c r="K86" s="17"/>
+      <c r="L86" s="17"/>
+      <c r="M86" s="17"/>
+      <c r="N86" s="17"/>
+      <c r="O86" s="17"/>
+      <c r="P86" s="17"/>
+      <c r="Q86" s="17"/>
+      <c r="R86" s="17"/>
+      <c r="S86" s="17"/>
+      <c r="T86" s="17"/>
+      <c r="U86" s="17"/>
+      <c r="V86" s="17"/>
+      <c r="W86" s="17"/>
+      <c r="X86" s="17"/>
+      <c r="Y86" s="17"/>
+      <c r="Z86" s="17"/>
+      <c r="AA86" s="17"/>
+      <c r="AB86" s="17"/>
+      <c r="AC86" s="17"/>
+      <c r="AD86" s="17"/>
+      <c r="AE86" s="17"/>
+      <c r="AF86" s="17"/>
+    </row>
+    <row r="87" spans="10:32">
+      <c r="M87" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S87" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V87" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W87" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y87" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB87" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC87" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD87" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF87" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="88" spans="10:32">
+      <c r="L88" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M88" s="1">
+        <v>3</v>
+      </c>
+      <c r="N88" s="1">
+        <v>1</v>
+      </c>
+      <c r="R88" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S88" s="8">
+        <v>2</v>
+      </c>
+      <c r="T88" s="8">
+        <v>2</v>
+      </c>
+      <c r="U88" s="8">
+        <v>2</v>
+      </c>
+      <c r="V88" s="8">
+        <v>2</v>
+      </c>
+      <c r="W88" s="8">
+        <v>2</v>
+      </c>
+      <c r="X88" s="8">
+        <v>2</v>
+      </c>
+      <c r="Y88" s="8">
+        <v>2</v>
+      </c>
+      <c r="Z88" s="8">
+        <v>2</v>
+      </c>
+      <c r="AA88" s="8">
+        <v>2</v>
+      </c>
+      <c r="AB88" s="8">
+        <v>2</v>
+      </c>
+      <c r="AC88" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD88" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE88" s="8">
+        <v>2</v>
+      </c>
+      <c r="AF88" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="10:32">
+      <c r="L89" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M89" s="1">
+        <v>2</v>
+      </c>
+      <c r="N89" s="1">
+        <v>0</v>
+      </c>
+      <c r="R89" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="S89" s="1">
+        <v>2</v>
+      </c>
+      <c r="T89" s="1">
+        <v>2</v>
+      </c>
+      <c r="U89" s="1">
+        <v>2</v>
+      </c>
+      <c r="V89" s="1">
+        <v>2</v>
+      </c>
+      <c r="W89" s="1">
+        <v>1</v>
+      </c>
+      <c r="X89" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y89" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="10:32">
+      <c r="L90" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M90" s="1">
+        <v>1</v>
+      </c>
+      <c r="N90" s="1">
+        <v>0</v>
+      </c>
+      <c r="R90" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="10:32">
+      <c r="R91" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="10:32">
+      <c r="R92" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="S92" s="1">
+        <v>1</v>
+      </c>
+      <c r="T92" s="1">
+        <v>1</v>
+      </c>
+      <c r="U92" s="1">
+        <v>1</v>
+      </c>
+      <c r="V92" s="1">
+        <v>1</v>
+      </c>
+      <c r="W92" s="1">
+        <v>1</v>
+      </c>
+      <c r="X92" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y92" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z92" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA92" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB92" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC92" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD92" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE92" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="10:32">
+      <c r="R93" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="95" spans="10:32">
+      <c r="S95" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T95" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V95" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W95" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y95" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB95" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC95" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD95" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF95" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="96" spans="10:32">
+      <c r="R96" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S96" s="8">
+        <v>2</v>
+      </c>
+      <c r="T96" s="8">
+        <v>2</v>
+      </c>
+      <c r="U96" s="8">
+        <v>2</v>
+      </c>
+      <c r="V96" s="8">
+        <v>2</v>
+      </c>
+      <c r="W96" s="8">
+        <v>0</v>
+      </c>
+      <c r="X96" s="8">
+        <v>1</v>
+      </c>
+      <c r="Y96" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z96" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA96" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB96" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC96" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD96" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE96" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF96" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="18:31">
+      <c r="R97" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="S97" s="1">
+        <v>0</v>
+      </c>
+      <c r="T97" s="1">
+        <v>0</v>
+      </c>
+      <c r="U97" s="1">
+        <v>0</v>
+      </c>
+      <c r="V97" s="1">
+        <v>1</v>
+      </c>
+      <c r="W97" s="1">
+        <v>2</v>
+      </c>
+      <c r="X97" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y97" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z97" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA97" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB97" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC97" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD97" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="18:31">
+      <c r="R98" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="18:31">
+      <c r="R99" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="18:31">
+      <c r="R100" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="101" spans="18:31">
+      <c r="R101" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>